<commit_message>
Final draft of User Stories
</commit_message>
<xml_diff>
--- a/Documents/Software Engineering Assignment Yr3.xlsx
+++ b/Documents/Software Engineering Assignment Yr3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28125"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noood\Desktop\year 2\Agile Semester 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="455" documentId="8_{B9C62D11-74F2-4B37-A0B2-6B12FF03A549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F4AFEF0-2930-46CA-81E3-1B74300C25FC}"/>
+  <xr:revisionPtr revIDLastSave="876" documentId="8_{B9C62D11-74F2-4B37-A0B2-6B12FF03A549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0C1133A-BFAE-48A2-B26E-6A92D7A7BE65}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="8" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="(Template)" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,10 @@
     <sheet name="Invoice" sheetId="7" r:id="rId3"/>
     <sheet name="Customer" sheetId="2" r:id="rId4"/>
     <sheet name="Order" sheetId="3" r:id="rId5"/>
-    <sheet name="Delivery Person" sheetId="4" r:id="rId6"/>
-    <sheet name="Delivery Docket" sheetId="5" r:id="rId7"/>
+    <sheet name="Delivery Docket" sheetId="5" r:id="rId6"/>
+    <sheet name="Delivery Person" sheetId="4" r:id="rId7"/>
+    <sheet name="Delivery Area" sheetId="8" r:id="rId8"/>
+    <sheet name="Address" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="162">
   <si>
     <t>Number</t>
   </si>
@@ -65,55 +67,58 @@
     <t xml:space="preserve">As a newsagent owner </t>
   </si>
   <si>
-    <t>Verify valid publication Name</t>
+    <t>Verify valid Publication ID 3 number ID</t>
   </si>
   <si>
     <t>I want to stock publications</t>
   </si>
   <si>
+    <t>Verify valid publication Name 1-64 characters</t>
+  </si>
+  <si>
+    <t>So I can provide my customers what they want</t>
+  </si>
+  <si>
     <t>Verify valid publication Type (Newspaper, Book, Magazine)</t>
   </si>
   <si>
-    <t>So I can provide my customers what they want</t>
-  </si>
-  <si>
-    <t>Verify publication frequency</t>
-  </si>
-  <si>
-    <t>verify total number to have in stock per day</t>
-  </si>
-  <si>
-    <t>Verify publication cost</t>
-  </si>
-  <si>
-    <t>Verify valid publiction</t>
+    <t xml:space="preserve">Verify publication frequency (Daily, Weekly, Fortnightly, Monthly, Once off(Books)) </t>
+  </si>
+  <si>
+    <t>verify total number to have in stock per day in range 0 - 100</t>
+  </si>
+  <si>
+    <t>Verify publication cost from min free(ie Galway advertiser) to max 50 euro</t>
+  </si>
+  <si>
+    <t>Verify invalid inputs are rejected and an appropriate error message is generated</t>
+  </si>
+  <si>
+    <t>Verify valid publiction as in User Story 1</t>
   </si>
   <si>
     <t>I want to view what publications I have availible</t>
   </si>
   <si>
-    <t>Verify valid publication in stock</t>
+    <t>Verify valid publication in stock from range 0 - 100</t>
   </si>
   <si>
     <t>So I can deliver whats ordered</t>
   </si>
   <si>
-    <t>Verify valid publiction as in User Story</t>
-  </si>
-  <si>
     <t>I want to update my publication Stock</t>
   </si>
   <si>
-    <t>Verify valid delivery of publications</t>
+    <t>Verify valid delivery of publications in range 0 - 100</t>
   </si>
   <si>
     <t>So I can manage my inventory</t>
   </si>
   <si>
-    <t>Verify update of stock</t>
-  </si>
-  <si>
-    <t>Verify valid empty stock</t>
+    <t>Verify update of stock min of 1</t>
+  </si>
+  <si>
+    <t>Verify valid empty stock of 0, none</t>
   </si>
   <si>
     <t>Verify valid publication as in User Story 1</t>
@@ -125,49 +130,22 @@
     <t>Verify publication deleted from catalogue</t>
   </si>
   <si>
-    <t>So I can have an up to date desirable publications</t>
-  </si>
-  <si>
-    <t>Verify publication is no longer in stock</t>
-  </si>
-  <si>
-    <t>As  a Customer</t>
-  </si>
-  <si>
-    <t>Verify vaild publication</t>
-  </si>
-  <si>
-    <t>I want to see what publications are availible</t>
-  </si>
-  <si>
-    <t>Verify publication in stock</t>
-  </si>
-  <si>
-    <t>So I can place an order</t>
-  </si>
-  <si>
-    <t>Verify can add to order</t>
-  </si>
-  <si>
-    <t>I want to update my order</t>
-  </si>
-  <si>
-    <t>So i can have additional reading material</t>
-  </si>
-  <si>
-    <t>Verify new total cost</t>
+    <t>So I can have an up to date list of desirable publications</t>
+  </si>
+  <si>
+    <t>Verify publication is no longer in stock of 0, none</t>
   </si>
   <si>
     <t>As a newsagent owner</t>
   </si>
   <si>
-    <t>Verify Customer Details</t>
+    <t>Verify Customer Details (name, address, orders, delivery area)</t>
   </si>
   <si>
     <t>I want to create a customer invoice at months end</t>
   </si>
   <si>
-    <t>Verify Customer total costs</t>
+    <t xml:space="preserve">Verify Customer total costs </t>
   </si>
   <si>
     <t>So I can manage my finances</t>
@@ -188,7 +166,7 @@
     <t>I want to view my customer invoice status</t>
   </si>
   <si>
-    <t>Verify Invoice status</t>
+    <t>Verify Invoice status paid, parialy paid or unpaid</t>
   </si>
   <si>
     <t>So I know who is paid or outstanding</t>
@@ -233,7 +211,7 @@
     <t>I want to create a customer</t>
   </si>
   <si>
-    <t>Verify valid address entered: 5-64 characters</t>
+    <t>Verify valid address entered: valid Address entity</t>
   </si>
   <si>
     <t>So I can manage my business</t>
@@ -245,7 +223,7 @@
     <t>Verify valid customer ID is generated for valid customer: Unique 1-6 digit number</t>
   </si>
   <si>
-    <t>Verify invalid inputs are rejected and an appropriate error message is generated</t>
+    <t>Verify valid customer status: Active/Paused (ie. holidays)</t>
   </si>
   <si>
     <t>Verify valid Customer ID entered: Existing customer ID</t>
@@ -260,19 +238,13 @@
     <t>I want to update a customer's details</t>
   </si>
   <si>
-    <t>Verify valid new name entered: 3-20 characters</t>
-  </si>
-  <si>
-    <t>Verify valid new address entered: 5-50 characters</t>
-  </si>
-  <si>
-    <t>Verify valid new phone number entered: 10-digit number</t>
-  </si>
-  <si>
-    <t>I want to delete a customer</t>
-  </si>
-  <si>
-    <t>Verify valid customer details removed as in User Story 1</t>
+    <t>Verify valid new details can be entered as in User Story 1</t>
+  </si>
+  <si>
+    <t>I want to archive a customer</t>
+  </si>
+  <si>
+    <t>Verify valid customer details from User Story 1 archived for 6 years</t>
   </si>
   <si>
     <t>Verify valid customer ID entered: Existing customer ID</t>
@@ -293,7 +265,7 @@
     <t>Verify valid total cost is calculated: Sum of individual publication costs</t>
   </si>
   <si>
-    <t>Verify valid order ID is generated:</t>
+    <t>Verify valid order ID is generated</t>
   </si>
   <si>
     <t>Verify valid order ID entered: Existing order ID</t>
@@ -329,7 +301,73 @@
     <t>I want to archive an order</t>
   </si>
   <si>
-    <t>...</t>
+    <t>Verify valid order details from User Story 1 archived for 6 years</t>
+  </si>
+  <si>
+    <t>As a news agent</t>
+  </si>
+  <si>
+    <t>Verify ID for every Delivery Docket - Unique code between 1-6 digits</t>
+  </si>
+  <si>
+    <t>I want to create a Delivery Docket</t>
+  </si>
+  <si>
+    <t>Verify the time order was delivered: Format 00:00</t>
+  </si>
+  <si>
+    <t>So that I can keep track of orders</t>
+  </si>
+  <si>
+    <t>Verify the delivery area for the order</t>
+  </si>
+  <si>
+    <t>Verify status if order is delivered: Y</t>
+  </si>
+  <si>
+    <t>Verify status if order is not delivered: N</t>
+  </si>
+  <si>
+    <t>Verify the list of orders needed for delivery</t>
+  </si>
+  <si>
+    <t>Verify the name of the customer on Docket - length 4-64 characters</t>
+  </si>
+  <si>
+    <t>Verify invalid imputs rejected. Error message appears</t>
+  </si>
+  <si>
+    <t>I want to read a Delivery Docket</t>
+  </si>
+  <si>
+    <t>Verify valid address: existing address</t>
+  </si>
+  <si>
+    <t>So that I can keep managing my business</t>
+  </si>
+  <si>
+    <t>Verify a new time for delivery if order is late: 00:00</t>
+  </si>
+  <si>
+    <t>I want to update a Delivery Docket</t>
+  </si>
+  <si>
+    <t>Verify new status on whether delivery has been delivered: Y/N</t>
+  </si>
+  <si>
+    <t>Verify new name of the customer on the Docket - length 4 - 64 characters</t>
+  </si>
+  <si>
+    <t>Verify that Delivery Docket Information in User Story 1 is perserved for future use</t>
+  </si>
+  <si>
+    <t>I want to archive a Delivery Docket</t>
+  </si>
+  <si>
+    <t>Verify that Delivery Docket Information in User Story 1 is accessible for 6 years.</t>
+  </si>
+  <si>
+    <t>so that I can perserve past orders</t>
   </si>
   <si>
     <t>Verify valid Name entered: 3-64 characters</t>
@@ -353,122 +391,152 @@
     <t>Verify that valid delivery person is assigned to one of 24 areas</t>
   </si>
   <si>
-    <t>Verify invalid name entered: 2 characters long 65+ characters long</t>
-  </si>
-  <si>
-    <t>Verify invalid age of delivery person: under 18 / over 75</t>
-  </si>
-  <si>
-    <t>Verify invalid phone number: e.g  0101014</t>
-  </si>
-  <si>
-    <t>Verify invalid stock?</t>
-  </si>
-  <si>
-    <t>Verify that age of Delivery person can be updated: 19- 75 years</t>
+    <t>Verify ID Verification number for each delivery person is generated. 1-6 digit number</t>
+  </si>
+  <si>
+    <t>Verify that age of Delivery person can be updated: 18 -75 years</t>
+  </si>
+  <si>
+    <t>I want to read a delivery person's details</t>
+  </si>
+  <si>
+    <t>Verify that the delivery docket can be updated</t>
+  </si>
+  <si>
+    <t>so that I a can manage my business</t>
+  </si>
+  <si>
+    <t>Verify that new phone number can be updated: 10-digit number</t>
+  </si>
+  <si>
+    <t>Verify valid new Name entered: 3-64 characters</t>
+  </si>
+  <si>
+    <t>Verify that delivery area can be updated</t>
   </si>
   <si>
     <t>I want to update a delivery person's details</t>
   </si>
   <si>
-    <t>Verify that the delivery docket can be updated</t>
+    <t>Verify that all details displayed in User Story 1 can be archived</t>
   </si>
   <si>
     <t>so that I can keep up to date with my delivery people</t>
   </si>
   <si>
-    <t>Verify that new phone number can be updated: 10-digit number</t>
-  </si>
-  <si>
-    <t>Verify valid new Name entered: 3-64 characters</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verify </t>
-  </si>
-  <si>
-    <t>I want to read a delivery person's details</t>
-  </si>
-  <si>
-    <t>so that I a can manage my business</t>
-  </si>
-  <si>
-    <t>Verify that all details displayed in User Story 1 can be deleted</t>
-  </si>
-  <si>
-    <t>I want to delete a delivery person</t>
-  </si>
-  <si>
-    <t>so that...</t>
-  </si>
-  <si>
-    <t>As a Delivery Person...</t>
-  </si>
-  <si>
-    <t>As a news agent</t>
-  </si>
-  <si>
-    <t>Verify the time order was delivered: Format 00:00</t>
-  </si>
-  <si>
-    <t>I want to create a Delivery Docket</t>
-  </si>
-  <si>
-    <t>Verify the delivery area for the order</t>
-  </si>
-  <si>
-    <t>So that I can keep track of orders</t>
-  </si>
-  <si>
-    <t>Verify status if order is delivered: Y</t>
-  </si>
-  <si>
-    <t>Verify status if order is not delivered: N</t>
-  </si>
-  <si>
-    <t>Verify the list of orders needed for delivery</t>
-  </si>
-  <si>
-    <t>Verify invalid time order was delivered: 000:00</t>
-  </si>
-  <si>
-    <t>Verify invalid delivery area for the order: Dublin</t>
-  </si>
-  <si>
-    <t>Verify that the</t>
-  </si>
-  <si>
-    <t>Verify a new time for delivery if order is late: 00:00</t>
-  </si>
-  <si>
-    <t>I want to update a Delivery Docket</t>
-  </si>
-  <si>
-    <t>Verify new status on whether delivery has been delivered: Y/N</t>
-  </si>
-  <si>
-    <t>I want to read a Delivery Docket</t>
-  </si>
-  <si>
-    <t>Verify valid address: existing address</t>
-  </si>
-  <si>
-    <t>So that I can keep managing my business</t>
-  </si>
-  <si>
-    <t>Verify that Delivery Docket Information in User Story 1 is perserved for future use</t>
-  </si>
-  <si>
-    <t>I want to archive a Delivery Docket</t>
-  </si>
-  <si>
-    <t>so that I can perserve past orders</t>
+    <t>Verify that Delivery Person Information in User Story 1 is accessible for 6 years.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that all information on the delivery person in User Story 1 is removed </t>
+  </si>
+  <si>
+    <t>I want to remove a delivery person</t>
+  </si>
+  <si>
+    <t>As they are no longer needed</t>
+  </si>
+  <si>
+    <t>Verify valid area id range 1-24</t>
+  </si>
+  <si>
+    <t>I want to create a delivery area</t>
+  </si>
+  <si>
+    <t>Verify valid delivery area entered 3-20 characters</t>
+  </si>
+  <si>
+    <t>so i can manage my busniess</t>
+  </si>
+  <si>
+    <t>verify each driver has their own area</t>
+  </si>
+  <si>
+    <t>Verify valid customer(name, address, active status, )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verify valid details as as user story 1 </t>
+  </si>
+  <si>
+    <t>I want to read the delivery area details</t>
+  </si>
+  <si>
+    <t>Verify access to list</t>
+  </si>
+  <si>
+    <t>So I can manage my delivery areas</t>
+  </si>
+  <si>
+    <t>as a newsagent</t>
+  </si>
+  <si>
+    <t>verify valid details as in user story 1 can be updated</t>
+  </si>
+  <si>
+    <t>i want to update the status of my delivery areas</t>
+  </si>
+  <si>
+    <t>so i can manage my business</t>
+  </si>
+  <si>
+    <t xml:space="preserve">as a newsagent </t>
+  </si>
+  <si>
+    <t>verify list archives</t>
+  </si>
+  <si>
+    <t>i want to archive delivery areas</t>
+  </si>
+  <si>
+    <t>verify valid delivery area is archived for 6 years</t>
+  </si>
+  <si>
+    <t>Verify valid postcode range 6-8</t>
+  </si>
+  <si>
+    <t>I want to log addresses</t>
+  </si>
+  <si>
+    <t>Verify valid street 3-20 characters</t>
+  </si>
+  <si>
+    <t>So that deliverys can be completed</t>
+  </si>
+  <si>
+    <t>Verify applicable house number range 1-4</t>
+  </si>
+  <si>
+    <t>Verify applicable house name 3-20 characters</t>
+  </si>
+  <si>
+    <t>Verify valid details displayed</t>
+  </si>
+  <si>
+    <t>I want to read addresses</t>
+  </si>
+  <si>
+    <t>So that deliverys are accurate</t>
+  </si>
+  <si>
+    <t>I want to update addresses</t>
+  </si>
+  <si>
+    <t>Verify list updates</t>
+  </si>
+  <si>
+    <t>I want to archive addresses</t>
+  </si>
+  <si>
+    <t>Verify valid address details are archived for 6 years</t>
+  </si>
+  <si>
+    <t>So that I can manage my business</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -493,13 +561,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -532,7 +593,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -544,20 +605,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -947,14 +1008,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C77332BC-ADED-4C2D-8CC5-9A86BA91BB27}">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="45.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="55.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="69.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -972,25 +1035,25 @@
       <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="3"/>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30.75">
+    <row r="5" spans="1:3">
       <c r="A5" s="3"/>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C5" t="s">
@@ -1007,149 +1070,133 @@
         <v>13</v>
       </c>
     </row>
+    <row r="8" spans="1:3">
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+    </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="3">
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="3">
         <v>2</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B11" t="s">
         <v>6</v>
       </c>
-      <c r="C9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
-      <c r="B11" t="s">
+    <row r="12" spans="1:3">
+      <c r="B12" t="s">
         <v>17</v>
       </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="3">
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="3">
         <v>3</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B15" t="s">
         <v>6</v>
       </c>
-      <c r="C13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="B14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="B16" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="B15" t="s">
+      <c r="C16" t="s">
         <v>21</v>
       </c>
-      <c r="C15" t="s">
+    </row>
+    <row r="17" spans="1:3">
+      <c r="B17" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="3">
-        <v>4</v>
-      </c>
-      <c r="B18" t="s">
-        <v>6</v>
-      </c>
       <c r="C18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
-      <c r="B19" t="s">
+    <row r="20" spans="1:3">
+      <c r="A20" s="3">
+        <v>4</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
         <v>25</v>
       </c>
-      <c r="C19" t="s">
+    </row>
+    <row r="21" spans="1:3">
+      <c r="B21" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="B20" t="s">
+      <c r="C21" t="s">
         <v>27</v>
       </c>
-      <c r="C20" t="s">
+    </row>
+    <row r="22" spans="1:3">
+      <c r="B22" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="3">
-        <v>5</v>
-      </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>29</v>
       </c>
-      <c r="C22" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="B23" t="s">
-        <v>31</v>
-      </c>
-      <c r="C23" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="B24" t="s">
-        <v>33</v>
-      </c>
-      <c r="C24" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="C25" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="11">
-        <v>6</v>
-      </c>
-      <c r="B27" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="12"/>
-      <c r="B28" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="12"/>
-      <c r="B29" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>37</v>
-      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="7"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="8"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="8"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="8"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="7"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="8"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="8"/>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="8"/>
+      <c r="B42" s="8"/>
+      <c r="C42" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1158,14 +1205,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E60E0919-244E-40AA-879A-A53D60A5695E}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="47.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1183,129 +1232,134 @@
       <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>39</v>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="3"/>
-      <c r="B4" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>41</v>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="3"/>
-      <c r="B5" s="4" t="s">
-        <v>42</v>
+      <c r="B5" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="C6" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="C7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="3">
         <v>2</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
         <v>38</v>
-      </c>
-      <c r="C9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="B10" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="B11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="3">
+        <v>39</v>
+      </c>
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="B12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="3">
         <v>3</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" t="s">
         <v>38</v>
-      </c>
-      <c r="C13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="B14" t="s">
-        <v>50</v>
-      </c>
-      <c r="C14" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="B15" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:3">
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
       <c r="C16" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="C17" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="C18" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="C19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="3">
         <v>4</v>
       </c>
-      <c r="B20" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
       <c r="B21" t="s">
-        <v>58</v>
+        <v>30</v>
       </c>
       <c r="C21" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="B22" t="s">
-        <v>42</v>
+        <v>50</v>
+      </c>
+      <c r="C22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="B23" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1317,14 +1371,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A0EA8BB-E26E-4E9C-BEB1-64FB15B65D62}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.85546875" customWidth="1"/>
+    <col min="2" max="2" width="35.140625" customWidth="1"/>
     <col min="3" max="3" width="74" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1343,61 +1397,66 @@
       <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>61</v>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="B4" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>63</v>
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="B5" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>65</v>
+      <c r="B5" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="C6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="C7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="C8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="3">
         <v>2</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" t="s">
         <v>60</v>
-      </c>
-      <c r="C9" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="B10" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="B11" t="s">
-        <v>64</v>
+        <v>61</v>
+      </c>
+      <c r="C11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="B12" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1405,36 +1464,26 @@
         <v>3</v>
       </c>
       <c r="B14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" t="s">
         <v>60</v>
-      </c>
-      <c r="C14" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="B15" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C15" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="B16" s="9" t="s">
-        <v>64</v>
+      <c r="B16" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="C16" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="C17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="C18" t="s">
-        <v>67</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -1442,23 +1491,23 @@
         <v>4</v>
       </c>
       <c r="B20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" t="s">
         <v>60</v>
-      </c>
-      <c r="C20" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="B21" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="C21" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="B22" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1470,15 +1519,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCD0ACF-20DA-45C9-B726-DA325D1ACDD6}">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.7109375" customWidth="1"/>
-    <col min="3" max="3" width="80" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" customWidth="1"/>
+    <col min="3" max="3" width="76.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1496,45 +1545,45 @@
       <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>77</v>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="B4" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>79</v>
+      <c r="B4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="B5" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>81</v>
+      <c r="B5" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="B6" s="7"/>
-      <c r="C6" s="6" t="s">
-        <v>82</v>
+      <c r="B6" s="5"/>
+      <c r="C6" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="B7" s="7"/>
+      <c r="B7" s="5"/>
       <c r="C7" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="B8" s="7"/>
-      <c r="C8" s="6" t="s">
-        <v>67</v>
+      <c r="B8" s="5"/>
+      <c r="C8" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1542,23 +1591,23 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C10" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="B11" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="C11" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="B12" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1566,41 +1615,41 @@
         <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C14" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="B15" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="C15" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="B16" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C16" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="C17" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="C18" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="C19" t="s">
-        <v>67</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -1608,23 +1657,23 @@
         <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C21" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="B22" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C22" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="B23" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1633,177 +1682,182 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E62DFE2D-2428-4D9E-B443-57322BE736A5}">
-  <dimension ref="A1:C57"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0991FD3-B03B-44F2-98CD-3E49EE4F5BC9}">
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="48.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="72.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="2" width="40.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="70.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1">
+    <row r="2" spans="1:4">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="B3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="B4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="B5"/>
+      <c r="C5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="B6"/>
+      <c r="C6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="B7"/>
+      <c r="C7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="B8"/>
+      <c r="C8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="B9"/>
+      <c r="C9" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="B4" s="1" t="s">
+    <row r="10" spans="1:4">
+      <c r="B10"/>
+      <c r="C10"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="2">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="B12" t="s">
         <v>97</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C12" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="B5" s="1" t="s">
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="B13" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C13"/>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="B14"/>
+      <c r="C14"/>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="2">
+        <v>3</v>
+      </c>
+      <c r="B15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="C6" s="1" t="s">
+    <row r="16" spans="1:4">
+      <c r="B16" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="C7" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="C8" s="1" t="s">
+      <c r="C16" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="C9" s="1" t="s">
+    <row r="17" spans="1:3">
+      <c r="B17" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
-      <c r="C10" s="1" t="s">
+    <row r="18" spans="1:3">
+      <c r="B18"/>
+      <c r="C18"/>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="2">
+        <v>4</v>
+      </c>
+      <c r="B19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
-      <c r="C11" s="1" t="s">
+    <row r="20" spans="1:3">
+      <c r="A20" s="3"/>
+      <c r="B20" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="C12" s="1" t="s">
+      <c r="C20" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="1">
-        <v>2</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C16" s="1" t="s">
+    <row r="21" spans="1:3">
+      <c r="A21" s="3"/>
+      <c r="B21" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="B17" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="B18" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="C19" s="10" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="C20" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="1">
-        <v>3</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="B33" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="B34" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" s="1">
-        <v>4</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2">
-      <c r="B49" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2">
-      <c r="B50" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2">
-      <c r="A57" s="1">
-        <v>5</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>119</v>
-      </c>
+      <c r="C21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1811,149 +1865,472 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0991FD3-B03B-44F2-98CD-3E49EE4F5BC9}">
-  <dimension ref="A1:C40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E62DFE2D-2428-4D9E-B443-57322BE736A5}">
+  <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="40.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="70.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="2" width="48.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="76.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="1">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="B4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="B5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="B6"/>
+      <c r="C6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="B7"/>
+      <c r="C7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="B8"/>
+      <c r="C8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="B9"/>
+      <c r="C9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="B10"/>
+      <c r="C10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="B11"/>
+      <c r="C11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="B12"/>
+      <c r="C12"/>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="2">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="B14" t="s">
+        <v>117</v>
+      </c>
+      <c r="C14" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="B15" t="s">
+        <v>119</v>
+      </c>
+      <c r="C15" t="s">
         <v>120</v>
       </c>
-      <c r="C3" s="1" t="s">
+    </row>
+    <row r="16" spans="1:3">
+      <c r="B16"/>
+      <c r="C16" s="6" t="s">
         <v>121</v>
       </c>
     </row>
+    <row r="17" spans="1:3">
+      <c r="B17"/>
+      <c r="C17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="B18"/>
+      <c r="C18"/>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="2">
+        <v>3</v>
+      </c>
+      <c r="B19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19"/>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="B20" t="s">
+        <v>123</v>
+      </c>
+      <c r="C20" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="B21" t="s">
+        <v>125</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="B22"/>
+      <c r="C22"/>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="2">
+        <v>4</v>
+      </c>
+      <c r="B23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="B24" t="s">
+        <v>128</v>
+      </c>
+      <c r="C24"/>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="B25" t="s">
+        <v>129</v>
+      </c>
+      <c r="C25"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E608B98C-1F0D-4731-BA23-5ACCAFA3CC66}">
+  <dimension ref="A1:C20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.5703125" customWidth="1"/>
+    <col min="3" max="3" width="73" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
+        <v>130</v>
+      </c>
+    </row>
     <row r="4" spans="1:3">
-      <c r="B4" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>123</v>
+      <c r="A4" s="3"/>
+      <c r="B4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C4" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="B5" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>125</v>
+      <c r="B5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C5" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="C6" s="1" t="s">
-        <v>126</v>
+      <c r="C6" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="C7" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="C8" s="1" t="s">
-        <v>128</v>
+      <c r="C7" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="C9" s="1" t="s">
-        <v>129</v>
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="C10" s="1" t="s">
-        <v>130</v>
+      <c r="B10" t="s">
+        <v>137</v>
+      </c>
+      <c r="C10" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="B11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>140</v>
+      </c>
+      <c r="C13" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="B14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="B15" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>144</v>
+      </c>
+      <c r="C18" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="1">
+      <c r="B19" t="s">
+        <v>146</v>
+      </c>
+      <c r="C19" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="B20" t="s">
+        <v>143</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B468A3D-86E5-4154-883D-45046BFFD781}">
+  <dimension ref="A1:C24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="33" customWidth="1"/>
+    <col min="3" max="3" width="47.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>131</v>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="3"/>
+      <c r="B4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="B5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="C6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="3">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="3"/>
+      <c r="B10" t="s">
+        <v>155</v>
+      </c>
+      <c r="C10" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="B11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="3">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="3"/>
+      <c r="B15" t="s">
+        <v>157</v>
+      </c>
+      <c r="C15" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="B16" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="3">
+        <v>3</v>
+      </c>
+      <c r="B19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="B20" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>133</v>
+      <c r="A20" s="3"/>
+      <c r="B20" t="s">
+        <v>159</v>
+      </c>
+      <c r="C20" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="B21" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="1">
-        <v>3</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="B27" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="B28" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="1">
-        <v>4</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="B39" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="B40" s="1" t="s">
-        <v>139</v>
-      </c>
+      <c r="B21" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="B24" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Reviewed User Stories document
</commit_message>
<xml_diff>
--- a/Documents/Software Engineering Assignment Yr3.xlsx
+++ b/Documents/Software Engineering Assignment Yr3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28125"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28122"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noood\Desktop\year 2\Agile Semester 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="876" documentId="8_{B9C62D11-74F2-4B37-A0B2-6B12FF03A549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0C1133A-BFAE-48A2-B26E-6A92D7A7BE65}"/>
+  <xr:revisionPtr revIDLastSave="952" documentId="8_{B9C62D11-74F2-4B37-A0B2-6B12FF03A549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F466F24F-A1D3-4785-BEA8-83442302753C}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="8" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="6" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="(Template)" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Delivery Docket" sheetId="5" r:id="rId6"/>
     <sheet name="Delivery Person" sheetId="4" r:id="rId7"/>
     <sheet name="Delivery Area" sheetId="8" r:id="rId8"/>
-    <sheet name="Address" sheetId="10" r:id="rId9"/>
+    <sheet name="Address (unused)" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="144">
   <si>
     <t>Number</t>
   </si>
@@ -67,7 +67,7 @@
     <t xml:space="preserve">As a newsagent owner </t>
   </si>
   <si>
-    <t>Verify valid Publication ID 3 number ID</t>
+    <t>Verify valid Publication ID: format PB 000, unique</t>
   </si>
   <si>
     <t>I want to stock publications</t>
@@ -133,7 +133,7 @@
     <t>So I can have an up to date list of desirable publications</t>
   </si>
   <si>
-    <t>Verify publication is no longer in stock of 0, none</t>
+    <t>Verify publication is no longer in stock  0, none</t>
   </si>
   <si>
     <t>As a newsagent owner</t>
@@ -160,13 +160,16 @@
     <t>Verify account cancelation if left unpaid for 3 months</t>
   </si>
   <si>
+    <t>Verify valid invoid ID: unique positive integer</t>
+  </si>
+  <si>
     <t>Verify valid invoice as in User Story One</t>
   </si>
   <si>
     <t>I want to view my customer invoice status</t>
   </si>
   <si>
-    <t>Verify Invoice status paid, parialy paid or unpaid</t>
+    <t>Verify Invoice status paid, partialy paid or unpaid</t>
   </si>
   <si>
     <t>So I know who is paid or outstanding</t>
@@ -199,7 +202,7 @@
     <t>I want to archive my invoices</t>
   </si>
   <si>
-    <t>Verify Invoice archived</t>
+    <t>Verify Invoice archived for 6 years</t>
   </si>
   <si>
     <t>As a newsagent</t>
@@ -226,27 +229,24 @@
     <t>Verify valid customer status: Active/Paused (ie. holidays)</t>
   </si>
   <si>
-    <t>Verify valid Customer ID entered: Existing customer ID</t>
+    <t>Verify valid details displayed as in User Story 1</t>
   </si>
   <si>
     <t>I want to read my customer's details</t>
   </si>
   <si>
-    <t>Verify valid details displayed as in User Story 1</t>
+    <t>Verify valid new details can be entered as in User Story 1</t>
   </si>
   <si>
     <t>I want to update a customer's details</t>
   </si>
   <si>
-    <t>Verify valid new details can be entered as in User Story 1</t>
+    <t>Verify valid customer details from User Story 1 archived for 6 years</t>
   </si>
   <si>
     <t>I want to archive a customer</t>
   </si>
   <si>
-    <t>Verify valid customer details from User Story 1 archived for 6 years</t>
-  </si>
-  <si>
     <t>Verify valid customer ID entered: Existing customer ID</t>
   </si>
   <si>
@@ -262,9 +262,6 @@
     <t>Verify valid day of week entered: Monday - Sunday</t>
   </si>
   <si>
-    <t>Verify valid total cost is calculated: Sum of individual publication costs</t>
-  </si>
-  <si>
     <t>Verify valid order ID is generated</t>
   </si>
   <si>
@@ -277,24 +274,15 @@
     <t>So I can check my deliveries</t>
   </si>
   <si>
+    <t>Verify valid details can be updated in User Story 1</t>
+  </si>
+  <si>
     <t>I want to update an order</t>
   </si>
   <si>
-    <t>Verify new valid customer ID entered</t>
-  </si>
-  <si>
     <t>So I can manage my deliveries</t>
   </si>
   <si>
-    <t>Verify new valid list of publications entered</t>
-  </si>
-  <si>
-    <t>Verify new valid day of week entered</t>
-  </si>
-  <si>
-    <t>Verify new valid total cost is calculated</t>
-  </si>
-  <si>
     <t>Verify valid order ID entered</t>
   </si>
   <si>
@@ -307,7 +295,7 @@
     <t>As a news agent</t>
   </si>
   <si>
-    <t>Verify ID for every Delivery Docket - Unique code between 1-6 digits</t>
+    <t>Verify ID for every Delivery Docket - Unique positive integer</t>
   </si>
   <si>
     <t>I want to create a Delivery Docket</t>
@@ -319,7 +307,7 @@
     <t>So that I can keep track of orders</t>
   </si>
   <si>
-    <t>Verify the delivery area for the order</t>
+    <t>Verify the delivery area for the docket</t>
   </si>
   <si>
     <t>Verify status if order is delivered: Y</t>
@@ -331,33 +319,18 @@
     <t>Verify the list of orders needed for delivery</t>
   </si>
   <si>
-    <t>Verify the name of the customer on Docket - length 4-64 characters</t>
-  </si>
-  <si>
-    <t>Verify invalid imputs rejected. Error message appears</t>
+    <t>Verify invalid inputs rejected. Error message appears</t>
   </si>
   <si>
     <t>I want to read a Delivery Docket</t>
   </si>
   <si>
-    <t>Verify valid address: existing address</t>
-  </si>
-  <si>
     <t>So that I can keep managing my business</t>
   </si>
   <si>
-    <t>Verify a new time for delivery if order is late: 00:00</t>
-  </si>
-  <si>
     <t>I want to update a Delivery Docket</t>
   </si>
   <si>
-    <t>Verify new status on whether delivery has been delivered: Y/N</t>
-  </si>
-  <si>
-    <t>Verify new name of the customer on the Docket - length 4 - 64 characters</t>
-  </si>
-  <si>
     <t>Verify that Delivery Docket Information in User Story 1 is perserved for future use</t>
   </si>
   <si>
@@ -376,67 +349,43 @@
     <t>i want to create delivery person</t>
   </si>
   <si>
-    <t>Verify that the stock is avaliable</t>
-  </si>
-  <si>
     <t>so I can deliver to different areas</t>
   </si>
   <si>
-    <t>Verify that the delivery docket has valid publications</t>
-  </si>
-  <si>
-    <t>Verify age of delivery person is entered: 18-75 years</t>
-  </si>
-  <si>
-    <t>Verify that valid delivery person is assigned to one of 24 areas</t>
-  </si>
-  <si>
-    <t>Verify ID Verification number for each delivery person is generated. 1-6 digit number</t>
-  </si>
-  <si>
-    <t>Verify that age of Delivery person can be updated: 18 -75 years</t>
+    <t>Verify that valid delivery person is assigned to valid delivery area</t>
+  </si>
+  <si>
+    <t>Verify ID Verification number for each delivery person is generated. Unique positive integer</t>
   </si>
   <si>
     <t>I want to read a delivery person's details</t>
   </si>
   <si>
-    <t>Verify that the delivery docket can be updated</t>
-  </si>
-  <si>
     <t>so that I a can manage my business</t>
   </si>
   <si>
-    <t>Verify that new phone number can be updated: 10-digit number</t>
-  </si>
-  <si>
-    <t>Verify valid new Name entered: 3-64 characters</t>
-  </si>
-  <si>
-    <t>Verify that delivery area can be updated</t>
+    <t>Verify valid details as in user story 1 can be updated</t>
   </si>
   <si>
     <t>I want to update a delivery person's details</t>
   </si>
   <si>
+    <t>so that I can keep up to date with my delivery people</t>
+  </si>
+  <si>
     <t>Verify that all details displayed in User Story 1 can be archived</t>
   </si>
   <si>
-    <t>so that I can keep up to date with my delivery people</t>
+    <t>I want to remove a delivery person</t>
   </si>
   <si>
     <t>Verify that Delivery Person Information in User Story 1 is accessible for 6 years.</t>
   </si>
   <si>
-    <t xml:space="preserve">Verify that all information on the delivery person in User Story 1 is removed </t>
-  </si>
-  <si>
-    <t>I want to remove a delivery person</t>
-  </si>
-  <si>
     <t>As they are no longer needed</t>
   </si>
   <si>
-    <t>Verify valid area id range 1-24</t>
+    <t>Verify valid area id: format AT000, unique</t>
   </si>
   <si>
     <t>I want to create a delivery area</t>
@@ -448,10 +397,7 @@
     <t>so i can manage my busniess</t>
   </si>
   <si>
-    <t>verify each driver has their own area</t>
-  </si>
-  <si>
-    <t>Verify valid customer(name, address, active status, )</t>
+    <t>Verify valid list of addresses</t>
   </si>
   <si>
     <t xml:space="preserve">verify valid details as as user story 1 </t>
@@ -593,7 +539,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -619,6 +565,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1011,7 +958,7 @@
   <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1205,7 +1152,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E60E0919-244E-40AA-879A-A53D60A5695E}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
@@ -1272,58 +1219,58 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="3">
+    <row r="9" spans="1:3">
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="3">
         <v>2</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>30</v>
       </c>
-      <c r="C10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>39</v>
-      </c>
-      <c r="C11" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="3">
+    <row r="13" spans="1:3">
+      <c r="B13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="3">
         <v>3</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>30</v>
       </c>
-      <c r="C14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="B15" t="s">
-        <v>42</v>
-      </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="B16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" t="s">
         <v>44</v>
       </c>
-      <c r="C16" t="s">
+    </row>
+    <row r="17" spans="1:3">
+      <c r="B17" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
       <c r="C17" t="s">
         <v>46</v>
       </c>
@@ -1338,27 +1285,32 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="3">
+    <row r="20" spans="1:3">
+      <c r="C20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="3">
         <v>4</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>30</v>
       </c>
-      <c r="C21" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>50</v>
-      </c>
-      <c r="C22" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="B23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="B24" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1369,10 +1321,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A0EA8BB-E26E-4E9C-BEB1-64FB15B65D62}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1398,31 +1350,31 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="B4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="B5" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="C6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1432,7 +1384,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="C8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1440,23 +1392,20 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C10" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="B11" t="s">
-        <v>61</v>
-      </c>
-      <c r="C11" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="B12" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1464,50 +1413,44 @@
         <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C14" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="B15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C15" t="s">
-        <v>64</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="B16" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C16" t="s">
-        <v>15</v>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="3">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="B19" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="3">
-        <v>4</v>
-      </c>
       <c r="B20" t="s">
-        <v>52</v>
-      </c>
-      <c r="C20" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="B21" t="s">
-        <v>65</v>
-      </c>
-      <c r="C21" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="B22" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1517,10 +1460,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCD0ACF-20DA-45C9-B726-DA325D1ACDD6}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1546,7 +1489,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C3" t="s">
         <v>67</v>
@@ -1577,103 +1520,82 @@
     <row r="7" spans="1:3">
       <c r="B7" s="5"/>
       <c r="C7" t="s">
-        <v>73</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="B8" s="5"/>
-      <c r="C8" t="s">
-        <v>15</v>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="3">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="3">
-        <v>2</v>
-      </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="C10" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="B11" t="s">
         <v>75</v>
       </c>
-      <c r="C11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="B12" t="s">
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="3">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="3">
-        <v>3</v>
-      </c>
       <c r="B14" t="s">
-        <v>52</v>
+        <v>77</v>
       </c>
       <c r="C14" t="s">
-        <v>74</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="B15" t="s">
-        <v>77</v>
-      </c>
-      <c r="C15" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
-      <c r="B16" t="s">
+    <row r="17" spans="1:3">
+      <c r="A17" s="3">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" t="s">
         <v>79</v>
       </c>
-      <c r="C16" t="s">
+    </row>
+    <row r="18" spans="1:3">
+      <c r="B18" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
-      <c r="C18" t="s">
-        <v>82</v>
-      </c>
-    </row>
     <row r="19" spans="1:3">
-      <c r="C19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="3">
-        <v>4</v>
-      </c>
-      <c r="B21" t="s">
-        <v>52</v>
-      </c>
-      <c r="C21" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="B22" t="s">
-        <v>84</v>
-      </c>
-      <c r="C22" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="B23" t="s">
-        <v>56</v>
+      <c r="B19" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1707,91 +1629,84 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="2">
+    <row r="3" spans="1:4">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
       <c r="B3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C3" t="s">
-        <v>89</v>
+        <v>82</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="B4" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C4" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="B5"/>
+      <c r="B5" t="s">
+        <v>86</v>
+      </c>
       <c r="C5" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="B6"/>
       <c r="C6" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="B7"/>
       <c r="C7" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="B8"/>
       <c r="C8" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="B9"/>
       <c r="C9" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="B10"/>
       <c r="C10"/>
+      <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2">
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4">
       <c r="B12" t="s">
-        <v>97</v>
-      </c>
-      <c r="C12" t="s">
-        <v>98</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="C12"/>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:4">
       <c r="B13" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C13"/>
       <c r="D13" s="1"/>
@@ -1799,34 +1714,31 @@
     <row r="14" spans="1:4">
       <c r="B14"/>
       <c r="C14"/>
-      <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2">
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C15" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="B16" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="C16" t="s">
-        <v>102</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="B17" t="s">
-        <v>90</v>
-      </c>
-      <c r="C17" t="s">
-        <v>103</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="C17"/>
     </row>
     <row r="18" spans="1:3">
       <c r="B18"/>
@@ -1837,25 +1749,25 @@
         <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C19" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="3"/>
       <c r="B20" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C20" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="3"/>
       <c r="B21" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="C21"/>
     </row>
@@ -1866,17 +1778,17 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E62DFE2D-2428-4D9E-B443-57322BE736A5}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2"/>
     <col min="2" max="2" width="48.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="76.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="83.140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1895,162 +1807,123 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C3" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="B4" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="C4" t="s">
-        <v>110</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="B5" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="C5" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="B6"/>
       <c r="C6" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="B7"/>
       <c r="C7" t="s">
-        <v>57</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="B8"/>
-      <c r="C8" t="s">
-        <v>114</v>
-      </c>
+      <c r="C8"/>
     </row>
     <row r="9" spans="1:3">
-      <c r="B9"/>
-      <c r="C9" t="s">
-        <v>115</v>
+      <c r="A9" s="2">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="B10"/>
-      <c r="C10" t="s">
-        <v>96</v>
-      </c>
+      <c r="B10" t="s">
+        <v>104</v>
+      </c>
+      <c r="C10"/>
     </row>
     <row r="11" spans="1:3">
-      <c r="B11"/>
-      <c r="C11" t="s">
-        <v>62</v>
-      </c>
+      <c r="B11" t="s">
+        <v>105</v>
+      </c>
+      <c r="C11"/>
     </row>
     <row r="12" spans="1:3">
       <c r="B12"/>
-      <c r="C12"/>
+      <c r="C12" s="6"/>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C13" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="B14" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="C14" t="s">
-        <v>118</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="B15" t="s">
-        <v>119</v>
-      </c>
-      <c r="C15" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="B16"/>
-      <c r="C16" s="6" t="s">
-        <v>121</v>
-      </c>
+      <c r="C16"/>
     </row>
     <row r="17" spans="1:3">
-      <c r="B17"/>
+      <c r="A17" s="2">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>53</v>
+      </c>
       <c r="C17" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="B18"/>
-      <c r="C18"/>
+      <c r="B18" t="s">
+        <v>110</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="2">
-        <v>3</v>
-      </c>
       <c r="B19" t="s">
-        <v>52</v>
+        <v>112</v>
       </c>
       <c r="C19"/>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="B20" t="s">
-        <v>123</v>
-      </c>
-      <c r="C20" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="B21" t="s">
-        <v>125</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="B22"/>
-      <c r="C22"/>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="2">
-        <v>4</v>
-      </c>
-      <c r="B23" t="s">
-        <v>52</v>
-      </c>
-      <c r="C23" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="B24" t="s">
-        <v>128</v>
-      </c>
-      <c r="C24"/>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="B25" t="s">
-        <v>129</v>
-      </c>
-      <c r="C25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2059,15 +1932,15 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E608B98C-1F0D-4731-BA23-5ACCAFA3CC66}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="48.5703125" customWidth="1"/>
     <col min="3" max="3" width="73" bestFit="1" customWidth="1"/>
   </cols>
@@ -2088,106 +1961,103 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C3" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="3"/>
       <c r="B4" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="C4" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="B5" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="C5" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="C6" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="C7" t="s">
         <v>15</v>
       </c>
     </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="3">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" t="s">
+        <v>118</v>
+      </c>
+    </row>
     <row r="9" spans="1:3">
-      <c r="A9">
-        <v>2</v>
-      </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>119</v>
       </c>
       <c r="C9" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="B10" t="s">
-        <v>137</v>
-      </c>
-      <c r="C10" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="B11" t="s">
-        <v>139</v>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="3">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>122</v>
+      </c>
+      <c r="C12" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13">
-        <v>3</v>
-      </c>
       <c r="B13" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="C13" t="s">
-        <v>141</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="B14" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="B15" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="3">
         <v>4</v>
       </c>
+      <c r="B16" t="s">
+        <v>126</v>
+      </c>
+      <c r="C16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="B17" t="s">
+        <v>128</v>
+      </c>
+      <c r="C17" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3">
       <c r="B18" t="s">
-        <v>144</v>
-      </c>
-      <c r="C18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="B19" t="s">
-        <v>146</v>
-      </c>
-      <c r="C19" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="B20" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -2197,7 +2067,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B468A3D-86E5-4154-883D-45046BFFD781}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
@@ -2205,9 +2075,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33" customWidth="1"/>
-    <col min="3" max="3" width="47.140625" customWidth="1"/>
+    <col min="3" max="3" width="69.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2226,32 +2096,37 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C3" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="3"/>
       <c r="B4" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="C4" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="B5" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="C5" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="C6" t="s">
-        <v>153</v>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="C7" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -2259,78 +2134,78 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C9" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="3"/>
       <c r="B10" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
       <c r="C10" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="B11" t="s">
-        <v>156</v>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="3">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="3">
-        <v>2</v>
-      </c>
+      <c r="A14" s="3"/>
       <c r="B14" t="s">
-        <v>52</v>
+        <v>139</v>
       </c>
       <c r="C14" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="3"/>
       <c r="B15" t="s">
-        <v>157</v>
-      </c>
-      <c r="C15" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="B16" t="s">
-        <v>156</v>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="3">
+        <v>3</v>
+      </c>
+      <c r="B17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="3"/>
+      <c r="B18" t="s">
+        <v>141</v>
+      </c>
+      <c r="C18" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="3">
-        <v>3</v>
-      </c>
       <c r="B19" t="s">
-        <v>52</v>
-      </c>
-      <c r="C19" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="3"/>
-      <c r="B20" t="s">
-        <v>159</v>
-      </c>
-      <c r="C20" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="B21" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="B24" s="1"/>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="B22" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>